<commit_message>
Update message design and Argument
</commit_message>
<xml_diff>
--- a/doc/MessageDesign.xlsx
+++ b/doc/MessageDesign.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19155" windowHeight="8520" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="19155" windowHeight="8520" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="4" r:id="rId1"/>
     <sheet name="Login,Register" sheetId="1" r:id="rId2"/>
     <sheet name="Friend" sheetId="2" r:id="rId3"/>
     <sheet name="Chat" sheetId="3" r:id="rId4"/>
+    <sheet name="Matching Game" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="91">
   <si>
     <t>Login</t>
   </si>
@@ -272,6 +273,24 @@
   </si>
   <si>
     <t>If failure</t>
+  </si>
+  <si>
+    <t>CMD_GAME_MATCHING</t>
+  </si>
+  <si>
+    <t>room_id</t>
+  </si>
+  <si>
+    <t>int(0,1)</t>
+  </si>
+  <si>
+    <t>0:fail,1:success</t>
+  </si>
+  <si>
+    <t>the room id user joined</t>
+  </si>
+  <si>
+    <t>Sau khi nhan message nay, player se nhan duoc message CMD_FRIEND_INFO</t>
   </si>
 </sst>
 </file>
@@ -882,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,8 +1718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,4 +1872,99 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
waiting room and chat system
</commit_message>
<xml_diff>
--- a/doc/MessageDesign.xlsx
+++ b/doc/MessageDesign.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19155" windowHeight="8520" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="19155" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="Format" sheetId="4" r:id="rId1"/>
@@ -779,7 +779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -1718,7 +1718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1879,7 +1879,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>